<commit_message>
new test results using new unit
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unsw-my.sharepoint.com/personal/z5244813_ad_unsw_edu_au/Documents/Computer Engineering/COMP4337/labs/COMP4337_labs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A38289F-5FC6-462E-BDEC-85771449023B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{7A38289F-5FC6-462E-BDEC-85771449023B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45ECDEBC-2F36-45FC-8ACF-CA4227FA116F}"/>
   <bookViews>
-    <workbookView xWindow="1550" yWindow="1040" windowWidth="28800" windowHeight="15460" xr2:uid="{9DC7044B-3D7B-4044-9FA0-12FADBE6C06D}"/>
+    <workbookView xWindow="3960" yWindow="3280" windowWidth="28800" windowHeight="15330" xr2:uid="{9DC7044B-3D7B-4044-9FA0-12FADBE6C06D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,23 +57,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>encryption</t>
+    <t>Present</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>decryption</t>
+    <t>encryption/μs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>digest generation</t>
+    <t>decryption/μs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>signature generation</t>
+    <t>digest generation/μs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Present</t>
+    <t>signature generation/μs</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -226,7 +226,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>encryption</c:v>
+                  <c:v>encryption/μs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -275,22 +275,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10020</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1E-3</c:v>
+                  <c:v>10020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1E-3</c:v>
+                  <c:v>10018</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1E-3</c:v>
+                  <c:v>10018</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1E-3</c:v>
+                  <c:v>10018</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1E-3</c:v>
+                  <c:v>10004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -310,7 +310,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>decryption</c:v>
+                  <c:v>decryption/μs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -359,22 +359,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1E-3</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1E-3</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1E-3</c:v>
+                  <c:v>10002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1E-3</c:v>
+                  <c:v>10002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1E-3</c:v>
+                  <c:v>10002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1E-3</c:v>
+                  <c:v>10012</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -673,7 +673,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>encryption</c:v>
+                  <c:v>encryption/μs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -740,16 +740,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1E-3</c:v>
+                  <c:v>10010</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>40038</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4E-2</c:v>
+                  <c:v>240224</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.188</c:v>
+                  <c:v>1881706</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -769,7 +769,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>decryption</c:v>
+                  <c:v>decryption/μs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -839,13 +839,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>30030</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.1000000000000001E-2</c:v>
+                  <c:v>220198</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.17199999999999999</c:v>
+                  <c:v>1711564</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1144,7 +1144,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>encryption</c:v>
+                  <c:v>encryption/μs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1214,13 +1214,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1E-3</c:v>
+                  <c:v>10006</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>30028</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.03</c:v>
+                  <c:v>290254</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1240,7 +1240,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>decryption</c:v>
+                  <c:v>decryption/μs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1307,16 +1307,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1E-3</c:v>
+                  <c:v>10014</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>30038</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.3E-2</c:v>
+                  <c:v>230204</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1623,7 +1623,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>digest generation</c:v>
+                  <c:v>digest generation/μs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1687,19 +1687,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1E-3</c:v>
+                  <c:v>9998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1E-3</c:v>
+                  <c:v>10008</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.01</c:v>
+                  <c:v>110092</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.10199999999999999</c:v>
+                  <c:v>1010914</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1975,7 +1975,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>signature generation</c:v>
+                  <c:v>signature generation/μs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2045,13 +2045,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1E-3</c:v>
+                  <c:v>10010</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>40028</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.3000000000000002E-2</c:v>
+                  <c:v>340302</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5434,12 +5434,12 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U27" sqref="U27"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="9" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5476,7 +5476,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -5491,21 +5491,21 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>1E-3</v>
+        <v>10010</v>
       </c>
       <c r="G3">
-        <v>4.0000000000000001E-3</v>
+        <v>40038</v>
       </c>
       <c r="H3">
-        <v>2.4E-2</v>
+        <v>240224</v>
       </c>
       <c r="I3">
-        <v>0.188</v>
+        <v>1881706</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -5523,13 +5523,13 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>3.0000000000000001E-3</v>
+        <v>30030</v>
       </c>
       <c r="H4">
-        <v>2.1000000000000001E-2</v>
+        <v>220198</v>
       </c>
       <c r="I4">
-        <v>0.17199999999999999</v>
+        <v>1711564</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -5565,7 +5565,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -5583,18 +5583,18 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>1E-3</v>
+        <v>10006</v>
       </c>
       <c r="H9">
-        <v>4.0000000000000001E-3</v>
+        <v>30028</v>
       </c>
       <c r="I9">
-        <v>0.03</v>
+        <v>290254</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -5609,16 +5609,16 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>1E-3</v>
+        <v>10014</v>
       </c>
       <c r="H10">
-        <v>3.0000000000000001E-3</v>
+        <v>30038</v>
       </c>
       <c r="I10">
-        <v>2.3E-2</v>
+        <v>230204</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -5648,48 +5648,48 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>10020</v>
       </c>
       <c r="C14">
-        <v>1E-3</v>
+        <v>10020</v>
       </c>
       <c r="D14">
-        <v>1E-3</v>
+        <v>10018</v>
       </c>
       <c r="E14">
-        <v>1E-3</v>
+        <v>10018</v>
       </c>
       <c r="F14">
-        <v>1E-3</v>
+        <v>10018</v>
       </c>
       <c r="G14">
-        <v>1E-3</v>
+        <v>10004</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B15">
-        <v>1E-3</v>
+        <v>10000</v>
       </c>
       <c r="C15">
-        <v>1E-3</v>
+        <v>10000</v>
       </c>
       <c r="D15">
-        <v>1E-3</v>
+        <v>10002</v>
       </c>
       <c r="E15">
-        <v>1E-3</v>
+        <v>10002</v>
       </c>
       <c r="F15">
-        <v>1E-3</v>
+        <v>10002</v>
       </c>
       <c r="G15">
-        <v>1E-3</v>
+        <v>10012</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -5725,7 +5725,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -5737,19 +5737,19 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>1E-3</v>
+        <v>9998</v>
       </c>
       <c r="G19">
-        <v>1E-3</v>
+        <v>10008</v>
       </c>
       <c r="H19">
-        <v>0.01</v>
+        <v>110092</v>
       </c>
       <c r="I19">
-        <v>0.10199999999999999</v>
+        <v>1010914</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -5785,7 +5785,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -5803,18 +5803,18 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <v>1E-3</v>
+        <v>10010</v>
       </c>
       <c r="H24">
-        <v>5.0000000000000001E-3</v>
+        <v>40028</v>
       </c>
       <c r="I24">
-        <v>3.3000000000000002E-2</v>
+        <v>340302</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>